<commit_message>
exhibitor with dummy content
</commit_message>
<xml_diff>
--- a/strapi/setup.xlsx
+++ b/strapi/setup.xlsx
@@ -5,83 +5,190 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Menu" sheetId="1" r:id="rId4"/>
+    <sheet name="exhibitor" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
-  <si>
-    <t>MenuName</t>
-  </si>
-  <si>
-    <t>MenuText</t>
-  </si>
-  <si>
-    <t>MenuIsVisible</t>
-  </si>
-  <si>
-    <t>MenuOrder</t>
-  </si>
-  <si>
-    <t>inspire</t>
-  </si>
-  <si>
-    <t>Inspire</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+  <si>
+    <t>Tabelle 1</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>isDeleted</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>internalComment</t>
+  </si>
+  <si>
+    <t>isReadOnly</t>
+  </si>
+  <si>
+    <t>dueDate</t>
+  </si>
+  <si>
+    <t>breakoutRoomUrl</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>contactEmail</t>
+  </si>
+  <si>
+    <t>contactName</t>
+  </si>
+  <si>
+    <t>contactPhone</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>disableSelfService</t>
+  </si>
+  <si>
+    <t>downloadFile1</t>
+  </si>
+  <si>
+    <t>downloadFile1Text</t>
+  </si>
+  <si>
+    <t>downloadFile2</t>
+  </si>
+  <si>
+    <t>downloadFile2Text</t>
+  </si>
+  <si>
+    <t>downloadFile3</t>
+  </si>
+  <si>
+    <t>downloadFile3Text</t>
+  </si>
+  <si>
+    <t>embeddedMedia</t>
+  </si>
+  <si>
+    <t>unavailableMessage</t>
+  </si>
+  <si>
+    <t>iFrameUrl</t>
+  </si>
+  <si>
+    <t>iFrameUrlLabel</t>
+  </si>
+  <si>
+    <t>isSponsor</t>
+  </si>
+  <si>
+    <t>isSponsorOnly</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>selfServiceEmail</t>
+  </si>
+  <si>
+    <t>selfServiceLink</t>
+  </si>
+  <si>
+    <t>showInteractions</t>
+  </si>
+  <si>
+    <t>sponsorBanner</t>
+  </si>
+  <si>
+    <t>tab1Html</t>
+  </si>
+  <si>
+    <t>tab1Label</t>
+  </si>
+  <si>
+    <t>tab2Html</t>
+  </si>
+  <si>
+    <t>tab2Label</t>
+  </si>
+  <si>
+    <t>tab3Html</t>
+  </si>
+  <si>
+    <t>tab3Label</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>HelloSpaces</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Die besten Spaces nur hier</t>
+  </si>
+  <si>
+    <t>Wetzlar</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="13"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>sven@efec.de</t>
+    </r>
+  </si>
+  <si>
+    <t>Sven Herchenhein</t>
+  </si>
+  <si>
+    <t>Deutschland</t>
+  </si>
+  <si>
+    <t>Connecting People &amp; Content</t>
+  </si>
+  <si>
+    <t>Wir sind zurzeit nicht erreichbar. Bitte versuchen sie es später noch einmal.</t>
   </si>
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>download</t>
-  </si>
-  <si>
-    <t>Download</t>
-  </si>
-  <si>
-    <t>upload</t>
-  </si>
-  <si>
-    <t>Upload</t>
-  </si>
-  <si>
-    <t>compare</t>
-  </si>
-  <si>
-    <t>Compare</t>
-  </si>
-  <si>
-    <t>view</t>
-  </si>
-  <si>
-    <t>View</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>home</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>wiki</t>
-  </si>
-  <si>
-    <t>Wiki</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="13"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://hellospaces.de/</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="d.m.yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -100,9 +207,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <u val="single"/>
       <sz val="10"/>
-      <color indexed="8"/>
+      <color indexed="13"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -126,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -154,12 +261,29 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -182,10 +306,29 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -203,54 +346,47 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -273,8 +409,8 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1339,152 +1475,712 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A2:AM14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="1" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="39" width="16.3516" style="1" customWidth="1"/>
+    <col min="40" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
+    <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="B2" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="C2" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="D2" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="Q2" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="R2" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="S2" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="T2" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="V2" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="W2" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="X2" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="Y2" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="Z2" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="AA2" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="AB2" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="AC2" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="AD2" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="AE2" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="AF2" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="AG2" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="AH2" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="AI2" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="AJ2" t="s" s="3">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s" s="3">
+        <v>37</v>
+      </c>
+      <c r="AL2" t="s" s="3">
+        <v>38</v>
+      </c>
+      <c r="AM2" t="s" s="3">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s" s="4">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5">
-        <v>2</v>
-      </c>
-      <c r="E2" s="6"/>
+    <row r="3" ht="50.25" customHeight="1">
+      <c r="A3" t="s" s="4">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s" s="5">
+        <v>41</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="F3" s="8">
+        <v>44187</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="I3" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="M3" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="N3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="Z3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" t="s" s="7">
+        <v>50</v>
+      </c>
+      <c r="AM3" s="6"/>
     </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D3" s="8">
-        <v>3</v>
-      </c>
-      <c r="E3" s="6"/>
+    <row r="4" ht="14.05" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="11"/>
+      <c r="AI4" s="11"/>
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="11"/>
+      <c r="AL4" s="11"/>
+      <c r="AM4" s="11"/>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D4" s="8">
-        <v>4</v>
-      </c>
-      <c r="E4" s="6"/>
+    <row r="5" ht="14.05" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="11"/>
+      <c r="AI5" s="11"/>
+      <c r="AJ5" s="11"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="11"/>
+      <c r="AM5" s="11"/>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D5" s="8">
-        <v>5</v>
-      </c>
-      <c r="E5" s="6"/>
+    <row r="6" ht="14.05" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="11"/>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D6" s="8">
-        <v>6</v>
-      </c>
-      <c r="E6" s="6"/>
+    <row r="7" ht="14.05" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="11"/>
+      <c r="AI7" s="11"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="11"/>
+      <c r="AM7" s="11"/>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D7" s="8">
-        <v>7</v>
-      </c>
-      <c r="E7" s="6"/>
+    <row r="8" ht="14.05" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="11"/>
+      <c r="AM8" s="11"/>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6"/>
+    <row r="9" ht="14.05" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="11"/>
+      <c r="AH9" s="11"/>
+      <c r="AI9" s="11"/>
+      <c r="AJ9" s="11"/>
+      <c r="AK9" s="11"/>
+      <c r="AL9" s="11"/>
+      <c r="AM9" s="11"/>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="9"/>
+    <row r="10" ht="14.05" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="11"/>
+      <c r="AM10" s="11"/>
+    </row>
+    <row r="11" ht="14.05" customHeight="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="11"/>
+      <c r="AM11" s="11"/>
+    </row>
+    <row r="12" ht="14.05" customHeight="1">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="11"/>
+      <c r="AG12" s="11"/>
+      <c r="AH12" s="11"/>
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="11"/>
+      <c r="AK12" s="11"/>
+      <c r="AL12" s="11"/>
+      <c r="AM12" s="11"/>
+    </row>
+    <row r="13" ht="14.05" customHeight="1">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="11"/>
+      <c r="AG13" s="11"/>
+      <c r="AH13" s="11"/>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="11"/>
+      <c r="AM13" s="11"/>
+    </row>
+    <row r="14" ht="14.05" customHeight="1">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="11"/>
+      <c r="AG14" s="11"/>
+      <c r="AH14" s="11"/>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="11"/>
+      <c r="AM14" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AM1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" location="" tooltip="" display="sven@efec.de"/>
+    <hyperlink ref="AL3" r:id="rId2" location="" tooltip="" display="https://hellospaces.de/"/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
schedule with dummy content
</commit_message>
<xml_diff>
--- a/strapi/setup.xlsx
+++ b/strapi/setup.xlsx
@@ -6,12 +6,13 @@
   </bookViews>
   <sheets>
     <sheet name="exhibitor" sheetId="1" r:id="rId4"/>
+    <sheet name="schedule" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
   <si>
     <t>Tabelle 1</t>
   </si>
@@ -181,6 +182,100 @@
       <t>https://hellospaces.de/</t>
     </r>
   </si>
+  <si>
+    <t>speakers</t>
+  </si>
+  <si>
+    <t>backgroundColor</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>channels</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>externalMeetingUrl</t>
+  </si>
+  <si>
+    <t>externalMeetingUrlButtonText</t>
+  </si>
+  <si>
+    <t>hasNoDetails</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>isMainSchedule</t>
+  </si>
+  <si>
+    <t>isBookable</t>
+  </si>
+  <si>
+    <t>mainCategory</t>
+  </si>
+  <si>
+    <t>mainItemUid</t>
+  </si>
+  <si>
+    <t>openInMainDirectly</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>textColor</t>
+  </si>
+  <si>
+    <t>videoUrl</t>
+  </si>
+  <si>
+    <t>zoomMeetingId</t>
+  </si>
+  <si>
+    <t>zoomMeetingPassword</t>
+  </si>
+  <si>
+    <t>zoomMeetingUrl</t>
+  </si>
+  <si>
+    <t>Willkommen</t>
+  </si>
+  <si>
+    <t>Willkommen auf der neuen Plattform</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>2021-01-01T12:00:00</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>+01:00</t>
+    </r>
+  </si>
+  <si>
+    <t>Beispieleintrag</t>
+  </si>
+  <si>
+    <t>live</t>
+  </si>
 </sst>
 </file>
 
@@ -190,7 +285,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="d.m.yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -210,6 +305,12 @@
       <u val="single"/>
       <sz val="10"/>
       <color indexed="13"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -352,7 +453,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -387,6 +488,21 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2187,4 +2303,303 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:AC6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B1" xSplit="1" ySplit="0" activePane="topRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="29" width="16.3516" style="12" customWidth="1"/>
+    <col min="30" max="256" width="16.3516" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.6" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+    </row>
+    <row r="2" ht="26.05" customHeight="1">
+      <c r="A2" t="s" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="14">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s" s="15">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s" s="15">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s" s="15">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s" s="15">
+        <v>55</v>
+      </c>
+      <c r="I2" t="s" s="15">
+        <v>56</v>
+      </c>
+      <c r="J2" t="s" s="15">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s" s="15">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s" s="15">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s" s="15">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s" s="15">
+        <v>60</v>
+      </c>
+      <c r="O2" t="s" s="15">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s" s="15">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s" s="15">
+        <v>62</v>
+      </c>
+      <c r="R2" t="s" s="15">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s" s="15">
+        <v>63</v>
+      </c>
+      <c r="T2" t="s" s="15">
+        <v>64</v>
+      </c>
+      <c r="U2" t="s" s="15">
+        <v>65</v>
+      </c>
+      <c r="V2" t="s" s="15">
+        <v>5</v>
+      </c>
+      <c r="W2" t="s" s="15">
+        <v>66</v>
+      </c>
+      <c r="X2" t="s" s="15">
+        <v>67</v>
+      </c>
+      <c r="Y2" t="s" s="15">
+        <v>3</v>
+      </c>
+      <c r="Z2" t="s" s="15">
+        <v>68</v>
+      </c>
+      <c r="AA2" t="s" s="15">
+        <v>69</v>
+      </c>
+      <c r="AB2" t="s" s="15">
+        <v>70</v>
+      </c>
+      <c r="AC2" t="s" s="15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" ht="26.05" customHeight="1">
+      <c r="A3" t="s" s="13">
+        <v>72</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="16">
+        <v>100</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" t="s" s="15">
+        <v>73</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" t="s" s="15">
+        <v>74</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" t="s" s="15">
+        <v>41</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" t="s" s="15">
+        <v>75</v>
+      </c>
+      <c r="P3" t="s" s="15">
+        <v>41</v>
+      </c>
+      <c r="Q3" t="s" s="15">
+        <v>49</v>
+      </c>
+      <c r="R3" t="s" s="15">
+        <v>41</v>
+      </c>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" t="s" s="15">
+        <v>49</v>
+      </c>
+      <c r="V3" t="s" s="15">
+        <v>41</v>
+      </c>
+      <c r="W3" t="s" s="15">
+        <v>76</v>
+      </c>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+    </row>
+    <row r="4" ht="14.05" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+    </row>
+    <row r="5" ht="14.05" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+    </row>
+    <row r="6" ht="14.05" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AC1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
stage with dummy content
</commit_message>
<xml_diff>
--- a/strapi/setup.xlsx
+++ b/strapi/setup.xlsx
@@ -7,12 +7,13 @@
   <sheets>
     <sheet name="exhibitor" sheetId="1" r:id="rId4"/>
     <sheet name="schedule" sheetId="2" r:id="rId5"/>
+    <sheet name="stage" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>Tabelle 1</t>
   </si>
@@ -275,6 +276,24 @@
   </si>
   <si>
     <t>live</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>isCrossLane</t>
+  </si>
+  <si>
+    <t>timetableOrder</t>
+  </si>
+  <si>
+    <t>viewOrder</t>
+  </si>
+  <si>
+    <t>Main Stage</t>
+  </si>
+  <si>
+    <t>Beispiel Main Stage</t>
   </si>
 </sst>
 </file>
@@ -453,7 +472,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -503,6 +522,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2602,4 +2630,227 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="12" width="16.3516" style="17" customWidth="1"/>
+    <col min="13" max="256" width="16.3516" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.6" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="3">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="3">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" t="s" s="4">
+        <v>81</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" t="s" s="7">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="H3" s="19">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="14.05" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+    </row>
+    <row r="5" ht="14.05" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" ht="14.05" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" ht="14.05" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" ht="14.05" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" ht="14.05" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" ht="14.05" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" ht="14.05" customHeight="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
speaker&vote with dummy content
</commit_message>
<xml_diff>
--- a/strapi/setup.xlsx
+++ b/strapi/setup.xlsx
@@ -8,12 +8,14 @@
     <sheet name="exhibitor" sheetId="1" r:id="rId4"/>
     <sheet name="schedule" sheetId="2" r:id="rId5"/>
     <sheet name="stage" sheetId="3" r:id="rId6"/>
+    <sheet name="speaker" sheetId="4" r:id="rId7"/>
+    <sheet name="vote" sheetId="5" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
   <si>
     <t>Tabelle 1</t>
   </si>
@@ -294,6 +296,81 @@
   </si>
   <si>
     <t>Beispiel Main Stage</t>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>companyImage</t>
+  </si>
+  <si>
+    <t>jobTitle</t>
+  </si>
+  <si>
+    <t>linkedInProfile</t>
+  </si>
+  <si>
+    <t>xingProfile</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>efec AG</t>
+  </si>
+  <si>
+    <t>Beispielspeaker</t>
+  </si>
+  <si>
+    <t>Studentischer Praktikant</t>
+  </si>
+  <si>
+    <t>answersClosed</t>
+  </si>
+  <si>
+    <t>isActive</t>
+  </si>
+  <si>
+    <t>option1</t>
+  </si>
+  <si>
+    <t>option2</t>
+  </si>
+  <si>
+    <t>option3</t>
+  </si>
+  <si>
+    <t>option4</t>
+  </si>
+  <si>
+    <t>option5</t>
+  </si>
+  <si>
+    <t>votingType</t>
+  </si>
+  <si>
+    <t>Voting</t>
+  </si>
+  <si>
+    <t>Beispielvoting</t>
+  </si>
+  <si>
+    <t>Super</t>
+  </si>
+  <si>
+    <t>Klasse</t>
+  </si>
+  <si>
+    <t>Toll</t>
+  </si>
+  <si>
+    <t>Fantastisch</t>
+  </si>
+  <si>
+    <t>Überragend</t>
   </si>
 </sst>
 </file>
@@ -472,7 +549,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -531,6 +608,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2853,4 +2936,590 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:Q11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="17" width="16.3516" style="20" customWidth="1"/>
+    <col min="18" max="256" width="16.3516" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.6" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s" s="3">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>87</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s" s="3">
+        <v>80</v>
+      </c>
+      <c r="Q2" t="s" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" ht="26.25" customHeight="1">
+      <c r="A3" t="s" s="4">
+        <v>89</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" t="s" s="7">
+        <v>90</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" t="s" s="7">
+        <v>91</v>
+      </c>
+      <c r="I3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s" s="7">
+        <v>92</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6"/>
+    </row>
+    <row r="4" ht="14.05" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+    </row>
+    <row r="5" ht="14.05" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" ht="14.05" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" ht="14.05" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" ht="14.05" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" ht="14.05" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" ht="14.05" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+    </row>
+    <row r="11" ht="14.05" customHeight="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:Q11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="17" width="16.3516" style="21" customWidth="1"/>
+    <col min="18" max="256" width="16.3516" style="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.6" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="3">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>96</v>
+      </c>
+      <c r="I2" t="s" s="3">
+        <v>97</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>98</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>99</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s" s="3">
+        <v>80</v>
+      </c>
+      <c r="Q2" t="s" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" t="s" s="4">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s" s="5">
+        <v>41</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" t="s" s="7">
+        <v>102</v>
+      </c>
+      <c r="E3" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s" s="7">
+        <v>103</v>
+      </c>
+      <c r="H3" t="s" s="7">
+        <v>104</v>
+      </c>
+      <c r="I3" t="s" s="7">
+        <v>105</v>
+      </c>
+      <c r="J3" t="s" s="7">
+        <v>106</v>
+      </c>
+      <c r="K3" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="L3" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6"/>
+    </row>
+    <row r="4" ht="14.05" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+    </row>
+    <row r="5" ht="14.05" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" ht="14.05" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" ht="14.05" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" ht="14.05" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" ht="14.05" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" ht="14.05" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+    </row>
+    <row r="11" ht="14.05" customHeight="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change exhibitor to expo
</commit_message>
<xml_diff>
--- a/strapi/setup.xlsx
+++ b/strapi/setup.xlsx
@@ -7,7 +7,7 @@
   <sheets>
     <sheet name="breakout" sheetId="1" r:id="rId4"/>
     <sheet name="contentitem" sheetId="2" r:id="rId5"/>
-    <sheet name="exhibitor" sheetId="3" r:id="rId6"/>
+    <sheet name="expo" sheetId="3" r:id="rId6"/>
     <sheet name="notification" sheetId="4" r:id="rId7"/>
     <sheet name="schedule" sheetId="5" r:id="rId8"/>
     <sheet name="speaker" sheetId="6" r:id="rId9"/>
@@ -204,7 +204,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="18"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>sven@efec.de</t>
@@ -230,7 +230,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="18"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://hellospaces.de/</t>
@@ -396,7 +396,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="18"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>christian@efec.de</t>
@@ -522,7 +522,7 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="18"/>
+      <color indexed="14"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -532,7 +532,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,20 +557,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="14"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="27">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -687,111 +675,6 @@
       <left style="thin">
         <color indexed="15"/>
       </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="19"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="10"/>
@@ -811,7 +694,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
@@ -821,10 +704,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
@@ -834,7 +717,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </left>
       <right/>
       <top/>
@@ -851,7 +734,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </right>
       <top/>
       <bottom/>
@@ -859,10 +742,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </right>
       <top/>
       <bottom/>
@@ -870,12 +753,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
@@ -884,31 +767,68 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="19"/>
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
@@ -918,7 +838,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -955,33 +875,6 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1012,6 +905,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1034,18 +948,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1091,10 +993,6 @@
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
@@ -2168,7 +2066,7 @@
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="12" width="16.3516" style="1" customWidth="1"/>
-    <col min="13" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1">
@@ -2365,96 +2263,96 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="11" width="16.3516" style="47" customWidth="1"/>
-    <col min="12" max="256" width="16.3516" style="47" customWidth="1"/>
+    <col min="1" max="11" width="16.3516" style="41" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="48">
+      <c r="A1" t="s" s="42">
         <v>115</v>
       </c>
-      <c r="B1" t="s" s="48">
+      <c r="B1" t="s" s="42">
         <v>5</v>
       </c>
-      <c r="C1" t="s" s="48">
+      <c r="C1" t="s" s="42">
         <v>6</v>
       </c>
-      <c r="D1" t="s" s="48">
+      <c r="D1" t="s" s="42">
         <v>89</v>
       </c>
-      <c r="E1" t="s" s="48">
+      <c r="E1" t="s" s="42">
         <v>104</v>
       </c>
-      <c r="F1" t="s" s="48">
+      <c r="F1" t="s" s="42">
         <v>116</v>
       </c>
-      <c r="G1" t="s" s="48">
+      <c r="G1" t="s" s="42">
         <v>91</v>
       </c>
-      <c r="H1" t="s" s="48">
+      <c r="H1" t="s" s="42">
         <v>117</v>
       </c>
-      <c r="I1" t="s" s="48">
+      <c r="I1" t="s" s="42">
         <v>82</v>
       </c>
-      <c r="J1" t="s" s="48">
+      <c r="J1" t="s" s="42">
         <v>8</v>
       </c>
-      <c r="K1" t="s" s="48">
+      <c r="K1" t="s" s="42">
         <v>20</v>
       </c>
     </row>
     <row r="2" ht="14.05" customHeight="1">
-      <c r="A2" t="s" s="27">
+      <c r="A2" t="s" s="18">
         <v>118</v>
       </c>
-      <c r="B2" t="s" s="28">
+      <c r="B2" t="s" s="19">
         <v>14</v>
       </c>
-      <c r="C2" t="s" s="29">
+      <c r="C2" t="s" s="20">
         <v>14</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="10"/>
-      <c r="J2" s="30">
+      <c r="J2" s="21">
         <v>1</v>
       </c>
       <c r="K2" s="10"/>
     </row>
     <row r="3" ht="14.05" customHeight="1">
-      <c r="A3" t="s" s="27">
+      <c r="A3" t="s" s="18">
         <v>119</v>
       </c>
-      <c r="B3" t="s" s="28">
+      <c r="B3" t="s" s="19">
         <v>14</v>
       </c>
-      <c r="C3" t="s" s="29">
+      <c r="C3" t="s" s="20">
         <v>14</v>
       </c>
-      <c r="D3" t="s" s="29">
+      <c r="D3" t="s" s="20">
         <v>98</v>
       </c>
-      <c r="E3" t="s" s="29">
+      <c r="E3" t="s" s="20">
         <v>107</v>
       </c>
-      <c r="F3" t="s" s="29">
+      <c r="F3" t="s" s="20">
         <v>97</v>
       </c>
-      <c r="G3" t="s" s="29">
+      <c r="G3" t="s" s="20">
         <v>120</v>
       </c>
-      <c r="H3" t="s" s="29">
+      <c r="H3" t="s" s="20">
         <v>121</v>
       </c>
       <c r="I3" s="10"/>
-      <c r="J3" s="30">
+      <c r="J3" s="21">
         <v>2</v>
       </c>
-      <c r="K3" t="s" s="29">
+      <c r="K3" t="s" s="20">
         <v>122</v>
       </c>
     </row>
@@ -2572,8 +2470,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="14" width="16.3516" style="49" customWidth="1"/>
-    <col min="15" max="256" width="16.3516" style="49" customWidth="1"/>
+    <col min="1" max="14" width="16.3516" style="43" customWidth="1"/>
+    <col min="15" max="16384" width="16.3516" style="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -2624,7 +2522,7 @@
       <c r="A2" t="s" s="3">
         <v>132</v>
       </c>
-      <c r="B2" t="s" s="22">
+      <c r="B2" t="s" s="13">
         <v>14</v>
       </c>
       <c r="C2" t="s" s="5">
@@ -2808,153 +2706,151 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="9" width="16.3516" style="11" customWidth="1"/>
-    <col min="10" max="256" width="16.3516" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="16.3516" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="12">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="12">
+      <c r="B1" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="C1" t="s" s="12">
+      <c r="C1" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="D1" t="s" s="12">
+      <c r="D1" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="E1" t="s" s="12">
+      <c r="E1" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="F1" t="s" s="12">
+      <c r="F1" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="G1" t="s" s="12">
+      <c r="G1" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="H1" t="s" s="12">
+      <c r="H1" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="I1" t="s" s="12">
+      <c r="I1" t="s" s="2">
         <v>22</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="13">
+      <c r="A2" t="s" s="3">
         <v>23</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" t="s" s="16">
+      <c r="B2" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="7">
         <v>1</v>
       </c>
-      <c r="F2" t="s" s="16">
+      <c r="F2" t="s" s="5">
         <v>25</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="17">
+      <c r="G2" s="6"/>
+      <c r="H2" s="7">
         <v>35</v>
       </c>
-      <c r="I2" s="15"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" ht="14.05" customHeight="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" ht="14.05" customHeight="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" ht="14.05" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" ht="14.05" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" ht="14.05" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" ht="14.05" customHeight="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" ht="14.05" customHeight="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -2976,8 +2872,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="36" width="16.3516" style="21" customWidth="1"/>
-    <col min="37" max="256" width="16.3516" style="21" customWidth="1"/>
+    <col min="1" max="36" width="16.3516" style="12" customWidth="1"/>
+    <col min="37" max="16384" width="16.3516" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -3094,7 +2990,7 @@
       <c r="A2" t="s" s="3">
         <v>57</v>
       </c>
-      <c r="B2" t="s" s="22">
+      <c r="B2" t="s" s="13">
         <v>14</v>
       </c>
       <c r="C2" t="s" s="5">
@@ -3598,8 +3494,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="23" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="23" customWidth="1"/>
+    <col min="1" max="7" width="16.3516" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -3626,7 +3522,7 @@
       </c>
     </row>
     <row r="2" ht="26.25" customHeight="1">
-      <c r="A2" t="s" s="24">
+      <c r="A2" t="s" s="15">
         <v>68</v>
       </c>
       <c r="B2" s="6"/>
@@ -3647,7 +3543,7 @@
       </c>
     </row>
     <row r="3" ht="14.05" customHeight="1">
-      <c r="A3" s="25"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -3656,7 +3552,7 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" ht="14.05" customHeight="1">
-      <c r="A4" s="25"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -3665,7 +3561,7 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" ht="14.05" customHeight="1">
-      <c r="A5" s="25"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -3674,7 +3570,7 @@
       <c r="G5" s="10"/>
     </row>
     <row r="6" ht="14.05" customHeight="1">
-      <c r="A6" s="25"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -3683,7 +3579,7 @@
       <c r="G6" s="10"/>
     </row>
     <row r="7" ht="14.05" customHeight="1">
-      <c r="A7" s="25"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -3692,7 +3588,7 @@
       <c r="G7" s="10"/>
     </row>
     <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -3701,7 +3597,7 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" ht="14.05" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -3710,7 +3606,7 @@
       <c r="G9" s="10"/>
     </row>
     <row r="10" ht="14.05" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -3732,137 +3628,137 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="26" width="16.3516" style="26" customWidth="1"/>
-    <col min="27" max="256" width="16.3516" style="26" customWidth="1"/>
+    <col min="1" max="26" width="16.3516" style="17" customWidth="1"/>
+    <col min="27" max="16384" width="16.3516" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.05" customHeight="1">
-      <c r="A1" t="s" s="27">
+      <c r="A1" t="s" s="18">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="28">
+      <c r="B1" t="s" s="19">
         <v>70</v>
       </c>
-      <c r="C1" t="s" s="29">
+      <c r="C1" t="s" s="20">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="29">
+      <c r="D1" t="s" s="20">
         <v>71</v>
       </c>
-      <c r="E1" t="s" s="29">
+      <c r="E1" t="s" s="20">
         <v>72</v>
       </c>
-      <c r="F1" t="s" s="29">
+      <c r="F1" t="s" s="20">
         <v>2</v>
       </c>
-      <c r="G1" t="s" s="29">
+      <c r="G1" t="s" s="20">
         <v>73</v>
       </c>
-      <c r="H1" t="s" s="29">
+      <c r="H1" t="s" s="20">
         <v>74</v>
       </c>
-      <c r="I1" t="s" s="29">
+      <c r="I1" t="s" s="20">
         <v>3</v>
       </c>
-      <c r="J1" t="s" s="29">
+      <c r="J1" t="s" s="20">
         <v>4</v>
       </c>
-      <c r="K1" t="s" s="29">
+      <c r="K1" t="s" s="20">
         <v>75</v>
       </c>
-      <c r="L1" t="s" s="29">
+      <c r="L1" t="s" s="20">
         <v>15</v>
       </c>
-      <c r="M1" t="s" s="29">
+      <c r="M1" t="s" s="20">
         <v>66</v>
       </c>
-      <c r="N1" t="s" s="29">
+      <c r="N1" t="s" s="20">
         <v>76</v>
       </c>
-      <c r="O1" t="s" s="29">
+      <c r="O1" t="s" s="20">
         <v>77</v>
       </c>
-      <c r="P1" t="s" s="29">
+      <c r="P1" t="s" s="20">
         <v>5</v>
       </c>
-      <c r="Q1" t="s" s="29">
+      <c r="Q1" t="s" s="20">
         <v>78</v>
       </c>
-      <c r="R1" t="s" s="29">
+      <c r="R1" t="s" s="20">
         <v>79</v>
       </c>
-      <c r="S1" t="s" s="29">
+      <c r="S1" t="s" s="20">
         <v>80</v>
       </c>
-      <c r="T1" t="s" s="29">
+      <c r="T1" t="s" s="20">
         <v>6</v>
       </c>
-      <c r="U1" t="s" s="29">
+      <c r="U1" t="s" s="20">
         <v>7</v>
       </c>
-      <c r="V1" t="s" s="29">
+      <c r="V1" t="s" s="20">
         <v>81</v>
       </c>
-      <c r="W1" t="s" s="29">
+      <c r="W1" t="s" s="20">
         <v>9</v>
       </c>
-      <c r="X1" t="s" s="29">
+      <c r="X1" t="s" s="20">
         <v>10</v>
       </c>
-      <c r="Y1" t="s" s="29">
+      <c r="Y1" t="s" s="20">
         <v>11</v>
       </c>
-      <c r="Z1" t="s" s="29">
+      <c r="Z1" t="s" s="20">
         <v>82</v>
       </c>
     </row>
     <row r="2" ht="26.05" customHeight="1">
-      <c r="A2" t="s" s="27">
+      <c r="A2" t="s" s="18">
         <v>83</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="30">
+      <c r="D2" s="21">
         <v>100</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" t="s" s="29">
+      <c r="F2" t="s" s="20">
         <v>84</v>
       </c>
-      <c r="G2" t="s" s="29">
+      <c r="G2" t="s" s="20">
         <v>85</v>
       </c>
-      <c r="H2" t="s" s="29">
+      <c r="H2" t="s" s="20">
         <v>86</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
-      <c r="K2" t="s" s="29">
+      <c r="K2" t="s" s="20">
         <v>14</v>
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
-      <c r="N2" t="s" s="29">
+      <c r="N2" t="s" s="20">
         <v>14</v>
       </c>
-      <c r="O2" t="s" s="29">
+      <c r="O2" t="s" s="20">
         <v>64</v>
       </c>
-      <c r="P2" t="s" s="29">
+      <c r="P2" t="s" s="20">
         <v>14</v>
       </c>
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
-      <c r="S2" t="s" s="29">
+      <c r="S2" t="s" s="20">
         <v>64</v>
       </c>
-      <c r="T2" t="s" s="29">
+      <c r="T2" t="s" s="20">
         <v>14</v>
       </c>
       <c r="U2" s="10"/>
@@ -3870,7 +3766,7 @@
       <c r="W2" s="10"/>
       <c r="X2" s="10"/>
       <c r="Y2" s="10"/>
-      <c r="Z2" t="s" s="29">
+      <c r="Z2" t="s" s="20">
         <v>87</v>
       </c>
     </row>
@@ -3959,116 +3855,144 @@
       <c r="Z5" s="10"/>
     </row>
     <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="33"/>
-      <c r="Z6" s="34"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="25"/>
     </row>
     <row r="7" ht="14.7" customHeight="1">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="36"/>
-      <c r="V7" s="36"/>
-      <c r="W7" s="36"/>
-      <c r="X7" s="36"/>
-      <c r="Y7" s="37"/>
-      <c r="Z7" s="38"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="29"/>
     </row>
     <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="36"/>
-      <c r="S8" s="36"/>
-      <c r="T8" s="36"/>
-      <c r="U8" s="36"/>
-      <c r="V8" s="36"/>
-      <c r="W8" s="36"/>
-      <c r="X8" s="36"/>
-      <c r="Y8" s="37"/>
-      <c r="Z8" s="38"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="27"/>
+      <c r="Y8" s="28"/>
+      <c r="Z8" s="29"/>
     </row>
     <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="39"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="40"/>
-      <c r="S9" s="40"/>
-      <c r="T9" s="40"/>
-      <c r="U9" s="40"/>
-      <c r="V9" s="40"/>
-      <c r="W9" s="40"/>
-      <c r="X9" s="40"/>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="42"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="33"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="34"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
+      <c r="X10" s="35"/>
+      <c r="Y10" s="35"/>
+      <c r="Z10" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -4090,8 +4014,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="17" width="16.3516" style="43" customWidth="1"/>
-    <col min="18" max="256" width="16.3516" style="43" customWidth="1"/>
+    <col min="1" max="17" width="16.3516" style="37" customWidth="1"/>
+    <col min="18" max="16384" width="16.3516" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -4350,8 +4274,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="9" width="16.3516" style="44" customWidth="1"/>
-    <col min="10" max="256" width="16.3516" style="44" customWidth="1"/>
+    <col min="1" max="9" width="16.3516" style="38" customWidth="1"/>
+    <col min="10" max="16384" width="16.3516" style="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -4514,8 +4438,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="8" width="16.3516" style="45" customWidth="1"/>
-    <col min="9" max="256" width="16.3516" style="45" customWidth="1"/>
+    <col min="1" max="8" width="16.3516" style="39" customWidth="1"/>
+    <col min="9" max="16384" width="16.3516" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -4545,7 +4469,7 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="24">
+      <c r="A2" t="s" s="15">
         <v>106</v>
       </c>
       <c r="B2" t="s" s="5">
@@ -4567,7 +4491,7 @@
       </c>
     </row>
     <row r="3" ht="14.05" customHeight="1">
-      <c r="A3" s="25"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -4577,7 +4501,7 @@
       <c r="H3" s="10"/>
     </row>
     <row r="4" ht="14.05" customHeight="1">
-      <c r="A4" s="25"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -4587,7 +4511,7 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" ht="14.05" customHeight="1">
-      <c r="A5" s="25"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -4597,7 +4521,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" ht="14.05" customHeight="1">
-      <c r="A6" s="25"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -4607,7 +4531,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" ht="14.05" customHeight="1">
-      <c r="A7" s="25"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -4617,7 +4541,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -4627,7 +4551,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" ht="14.05" customHeight="1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -4637,7 +4561,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" ht="14.05" customHeight="1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -4669,8 +4593,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="13" width="16.3516" style="46" customWidth="1"/>
-    <col min="14" max="256" width="16.3516" style="46" customWidth="1"/>
+    <col min="1" max="13" width="16.3516" style="40" customWidth="1"/>
+    <col min="14" max="16384" width="16.3516" style="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">

</xml_diff>